<commit_message>
Refactor CSS: Create Simple.css
</commit_message>
<xml_diff>
--- a/www/Scripts/ts/User/Levels.xlsx
+++ b/www/Scripts/ts/User/Levels.xlsx
@@ -476,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M80"/>
+  <dimension ref="A1:M100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I92" sqref="I5:I92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4354,6 +4354,738 @@
         <f t="shared" si="60"/>
         <v>225</v>
       </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="str">
+        <f t="shared" ref="A81:A100" si="63">"W"&amp;B81&amp;"L"&amp;C81</f>
+        <v>W12L1</v>
+      </c>
+      <c r="B81" s="1">
+        <f t="shared" ref="B81:B100" si="64">IF(OR(C80&lt;$B$1+1,C80&lt;B80),B80,B80+1)</f>
+        <v>12</v>
+      </c>
+      <c r="C81" s="1">
+        <f t="shared" ref="C81:C100" si="65">IF(B80=B81,C80+1,1)</f>
+        <v>1</v>
+      </c>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1">
+        <f t="shared" ref="E81:E100" si="66">B81</f>
+        <v>12</v>
+      </c>
+      <c r="F81" s="1">
+        <f t="shared" ref="F81:F100" si="67">E81+$B$1</f>
+        <v>16</v>
+      </c>
+      <c r="G81" s="1">
+        <f t="shared" ref="G81:G100" si="68">C81</f>
+        <v>1</v>
+      </c>
+      <c r="H81" s="1">
+        <f t="shared" ref="H81:H100" si="69">G81+$B$1</f>
+        <v>5</v>
+      </c>
+      <c r="I81" s="1" t="str">
+        <f t="shared" ref="I81:I100" si="70">"+'"&amp;A81&amp;" "&amp;B81&amp;" "&amp;C81&amp;" "&amp;D81&amp;" "&amp;E81&amp;" "&amp;F81&amp;" "&amp;G81&amp;" "&amp;H81&amp;" \r\n'"</f>
+        <v>+'W12L1 12 1  12 16 1 5 \r\n'</v>
+      </c>
+      <c r="J81" s="1">
+        <f t="shared" ref="J81:J100" si="71">E81*G81</f>
+        <v>12</v>
+      </c>
+      <c r="K81" s="1">
+        <f t="shared" ref="K81:K100" si="72">E81*H81</f>
+        <v>60</v>
+      </c>
+      <c r="L81" s="1">
+        <f t="shared" ref="L81:L100" si="73">F81*G81</f>
+        <v>16</v>
+      </c>
+      <c r="M81" s="1">
+        <f t="shared" ref="M81:M100" si="74">F81*H81</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="str">
+        <f t="shared" si="63"/>
+        <v>W12L2</v>
+      </c>
+      <c r="B82" s="1">
+        <f t="shared" si="64"/>
+        <v>12</v>
+      </c>
+      <c r="C82" s="1">
+        <f t="shared" si="65"/>
+        <v>2</v>
+      </c>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1">
+        <f t="shared" si="66"/>
+        <v>12</v>
+      </c>
+      <c r="F82" s="1">
+        <f t="shared" si="67"/>
+        <v>16</v>
+      </c>
+      <c r="G82" s="1">
+        <f t="shared" si="68"/>
+        <v>2</v>
+      </c>
+      <c r="H82" s="1">
+        <f t="shared" si="69"/>
+        <v>6</v>
+      </c>
+      <c r="I82" s="1" t="str">
+        <f t="shared" si="70"/>
+        <v>+'W12L2 12 2  12 16 2 6 \r\n'</v>
+      </c>
+      <c r="J82" s="1">
+        <f t="shared" si="71"/>
+        <v>24</v>
+      </c>
+      <c r="K82" s="1">
+        <f t="shared" si="72"/>
+        <v>72</v>
+      </c>
+      <c r="L82" s="1">
+        <f t="shared" si="73"/>
+        <v>32</v>
+      </c>
+      <c r="M82" s="1">
+        <f t="shared" si="74"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="str">
+        <f t="shared" si="63"/>
+        <v>W12L3</v>
+      </c>
+      <c r="B83" s="1">
+        <f t="shared" si="64"/>
+        <v>12</v>
+      </c>
+      <c r="C83" s="1">
+        <f t="shared" si="65"/>
+        <v>3</v>
+      </c>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1">
+        <f t="shared" si="66"/>
+        <v>12</v>
+      </c>
+      <c r="F83" s="1">
+        <f t="shared" si="67"/>
+        <v>16</v>
+      </c>
+      <c r="G83" s="1">
+        <f t="shared" si="68"/>
+        <v>3</v>
+      </c>
+      <c r="H83" s="1">
+        <f t="shared" si="69"/>
+        <v>7</v>
+      </c>
+      <c r="I83" s="1" t="str">
+        <f t="shared" si="70"/>
+        <v>+'W12L3 12 3  12 16 3 7 \r\n'</v>
+      </c>
+      <c r="J83" s="1">
+        <f t="shared" si="71"/>
+        <v>36</v>
+      </c>
+      <c r="K83" s="1">
+        <f t="shared" si="72"/>
+        <v>84</v>
+      </c>
+      <c r="L83" s="1">
+        <f t="shared" si="73"/>
+        <v>48</v>
+      </c>
+      <c r="M83" s="1">
+        <f t="shared" si="74"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="str">
+        <f t="shared" si="63"/>
+        <v>W12L4</v>
+      </c>
+      <c r="B84" s="1">
+        <f t="shared" si="64"/>
+        <v>12</v>
+      </c>
+      <c r="C84" s="1">
+        <f t="shared" si="65"/>
+        <v>4</v>
+      </c>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1">
+        <f t="shared" si="66"/>
+        <v>12</v>
+      </c>
+      <c r="F84" s="1">
+        <f t="shared" si="67"/>
+        <v>16</v>
+      </c>
+      <c r="G84" s="1">
+        <f t="shared" si="68"/>
+        <v>4</v>
+      </c>
+      <c r="H84" s="1">
+        <f t="shared" si="69"/>
+        <v>8</v>
+      </c>
+      <c r="I84" s="1" t="str">
+        <f t="shared" si="70"/>
+        <v>+'W12L4 12 4  12 16 4 8 \r\n'</v>
+      </c>
+      <c r="J84" s="1">
+        <f t="shared" si="71"/>
+        <v>48</v>
+      </c>
+      <c r="K84" s="1">
+        <f t="shared" si="72"/>
+        <v>96</v>
+      </c>
+      <c r="L84" s="1">
+        <f t="shared" si="73"/>
+        <v>64</v>
+      </c>
+      <c r="M84" s="1">
+        <f t="shared" si="74"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="str">
+        <f t="shared" si="63"/>
+        <v>W12L5</v>
+      </c>
+      <c r="B85" s="1">
+        <f t="shared" si="64"/>
+        <v>12</v>
+      </c>
+      <c r="C85" s="1">
+        <f t="shared" si="65"/>
+        <v>5</v>
+      </c>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1">
+        <f t="shared" si="66"/>
+        <v>12</v>
+      </c>
+      <c r="F85" s="1">
+        <f t="shared" si="67"/>
+        <v>16</v>
+      </c>
+      <c r="G85" s="1">
+        <f t="shared" si="68"/>
+        <v>5</v>
+      </c>
+      <c r="H85" s="1">
+        <f t="shared" si="69"/>
+        <v>9</v>
+      </c>
+      <c r="I85" s="1" t="str">
+        <f t="shared" si="70"/>
+        <v>+'W12L5 12 5  12 16 5 9 \r\n'</v>
+      </c>
+      <c r="J85" s="1">
+        <f t="shared" si="71"/>
+        <v>60</v>
+      </c>
+      <c r="K85" s="1">
+        <f t="shared" si="72"/>
+        <v>108</v>
+      </c>
+      <c r="L85" s="1">
+        <f t="shared" si="73"/>
+        <v>80</v>
+      </c>
+      <c r="M85" s="1">
+        <f t="shared" si="74"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="str">
+        <f t="shared" si="63"/>
+        <v>W12L6</v>
+      </c>
+      <c r="B86" s="1">
+        <f t="shared" si="64"/>
+        <v>12</v>
+      </c>
+      <c r="C86" s="1">
+        <f t="shared" si="65"/>
+        <v>6</v>
+      </c>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1">
+        <f t="shared" si="66"/>
+        <v>12</v>
+      </c>
+      <c r="F86" s="1">
+        <f t="shared" si="67"/>
+        <v>16</v>
+      </c>
+      <c r="G86" s="1">
+        <f t="shared" si="68"/>
+        <v>6</v>
+      </c>
+      <c r="H86" s="1">
+        <f t="shared" si="69"/>
+        <v>10</v>
+      </c>
+      <c r="I86" s="1" t="str">
+        <f t="shared" si="70"/>
+        <v>+'W12L6 12 6  12 16 6 10 \r\n'</v>
+      </c>
+      <c r="J86" s="1">
+        <f t="shared" si="71"/>
+        <v>72</v>
+      </c>
+      <c r="K86" s="1">
+        <f t="shared" si="72"/>
+        <v>120</v>
+      </c>
+      <c r="L86" s="1">
+        <f t="shared" si="73"/>
+        <v>96</v>
+      </c>
+      <c r="M86" s="1">
+        <f t="shared" si="74"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="str">
+        <f t="shared" si="63"/>
+        <v>W12L7</v>
+      </c>
+      <c r="B87" s="1">
+        <f t="shared" si="64"/>
+        <v>12</v>
+      </c>
+      <c r="C87" s="1">
+        <f t="shared" si="65"/>
+        <v>7</v>
+      </c>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1">
+        <f t="shared" si="66"/>
+        <v>12</v>
+      </c>
+      <c r="F87" s="1">
+        <f t="shared" si="67"/>
+        <v>16</v>
+      </c>
+      <c r="G87" s="1">
+        <f t="shared" si="68"/>
+        <v>7</v>
+      </c>
+      <c r="H87" s="1">
+        <f t="shared" si="69"/>
+        <v>11</v>
+      </c>
+      <c r="I87" s="1" t="str">
+        <f t="shared" si="70"/>
+        <v>+'W12L7 12 7  12 16 7 11 \r\n'</v>
+      </c>
+      <c r="J87" s="1">
+        <f t="shared" si="71"/>
+        <v>84</v>
+      </c>
+      <c r="K87" s="1">
+        <f t="shared" si="72"/>
+        <v>132</v>
+      </c>
+      <c r="L87" s="1">
+        <f t="shared" si="73"/>
+        <v>112</v>
+      </c>
+      <c r="M87" s="1">
+        <f t="shared" si="74"/>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="str">
+        <f t="shared" si="63"/>
+        <v>W12L8</v>
+      </c>
+      <c r="B88" s="1">
+        <f t="shared" si="64"/>
+        <v>12</v>
+      </c>
+      <c r="C88" s="1">
+        <f t="shared" si="65"/>
+        <v>8</v>
+      </c>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1">
+        <f t="shared" si="66"/>
+        <v>12</v>
+      </c>
+      <c r="F88" s="1">
+        <f t="shared" si="67"/>
+        <v>16</v>
+      </c>
+      <c r="G88" s="1">
+        <f t="shared" si="68"/>
+        <v>8</v>
+      </c>
+      <c r="H88" s="1">
+        <f t="shared" si="69"/>
+        <v>12</v>
+      </c>
+      <c r="I88" s="1" t="str">
+        <f t="shared" si="70"/>
+        <v>+'W12L8 12 8  12 16 8 12 \r\n'</v>
+      </c>
+      <c r="J88" s="1">
+        <f t="shared" si="71"/>
+        <v>96</v>
+      </c>
+      <c r="K88" s="1">
+        <f t="shared" si="72"/>
+        <v>144</v>
+      </c>
+      <c r="L88" s="1">
+        <f t="shared" si="73"/>
+        <v>128</v>
+      </c>
+      <c r="M88" s="1">
+        <f t="shared" si="74"/>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="str">
+        <f t="shared" si="63"/>
+        <v>W12L9</v>
+      </c>
+      <c r="B89" s="1">
+        <f t="shared" si="64"/>
+        <v>12</v>
+      </c>
+      <c r="C89" s="1">
+        <f t="shared" si="65"/>
+        <v>9</v>
+      </c>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1">
+        <f t="shared" si="66"/>
+        <v>12</v>
+      </c>
+      <c r="F89" s="1">
+        <f t="shared" si="67"/>
+        <v>16</v>
+      </c>
+      <c r="G89" s="1">
+        <f t="shared" si="68"/>
+        <v>9</v>
+      </c>
+      <c r="H89" s="1">
+        <f t="shared" si="69"/>
+        <v>13</v>
+      </c>
+      <c r="I89" s="1" t="str">
+        <f t="shared" si="70"/>
+        <v>+'W12L9 12 9  12 16 9 13 \r\n'</v>
+      </c>
+      <c r="J89" s="1">
+        <f t="shared" si="71"/>
+        <v>108</v>
+      </c>
+      <c r="K89" s="1">
+        <f t="shared" si="72"/>
+        <v>156</v>
+      </c>
+      <c r="L89" s="1">
+        <f t="shared" si="73"/>
+        <v>144</v>
+      </c>
+      <c r="M89" s="1">
+        <f t="shared" si="74"/>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="str">
+        <f t="shared" si="63"/>
+        <v>W12L10</v>
+      </c>
+      <c r="B90" s="1">
+        <f t="shared" si="64"/>
+        <v>12</v>
+      </c>
+      <c r="C90" s="1">
+        <f t="shared" si="65"/>
+        <v>10</v>
+      </c>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1">
+        <f t="shared" si="66"/>
+        <v>12</v>
+      </c>
+      <c r="F90" s="1">
+        <f t="shared" si="67"/>
+        <v>16</v>
+      </c>
+      <c r="G90" s="1">
+        <f t="shared" si="68"/>
+        <v>10</v>
+      </c>
+      <c r="H90" s="1">
+        <f t="shared" si="69"/>
+        <v>14</v>
+      </c>
+      <c r="I90" s="1" t="str">
+        <f t="shared" si="70"/>
+        <v>+'W12L10 12 10  12 16 10 14 \r\n'</v>
+      </c>
+      <c r="J90" s="1">
+        <f t="shared" si="71"/>
+        <v>120</v>
+      </c>
+      <c r="K90" s="1">
+        <f t="shared" si="72"/>
+        <v>168</v>
+      </c>
+      <c r="L90" s="1">
+        <f t="shared" si="73"/>
+        <v>160</v>
+      </c>
+      <c r="M90" s="1">
+        <f t="shared" si="74"/>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="str">
+        <f t="shared" si="63"/>
+        <v>W12L11</v>
+      </c>
+      <c r="B91" s="1">
+        <f t="shared" si="64"/>
+        <v>12</v>
+      </c>
+      <c r="C91" s="1">
+        <f t="shared" si="65"/>
+        <v>11</v>
+      </c>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1">
+        <f t="shared" si="66"/>
+        <v>12</v>
+      </c>
+      <c r="F91" s="1">
+        <f t="shared" si="67"/>
+        <v>16</v>
+      </c>
+      <c r="G91" s="1">
+        <f t="shared" si="68"/>
+        <v>11</v>
+      </c>
+      <c r="H91" s="1">
+        <f t="shared" si="69"/>
+        <v>15</v>
+      </c>
+      <c r="I91" s="1" t="str">
+        <f t="shared" si="70"/>
+        <v>+'W12L11 12 11  12 16 11 15 \r\n'</v>
+      </c>
+      <c r="J91" s="1">
+        <f t="shared" si="71"/>
+        <v>132</v>
+      </c>
+      <c r="K91" s="1">
+        <f t="shared" si="72"/>
+        <v>180</v>
+      </c>
+      <c r="L91" s="1">
+        <f t="shared" si="73"/>
+        <v>176</v>
+      </c>
+      <c r="M91" s="1">
+        <f t="shared" si="74"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="str">
+        <f t="shared" si="63"/>
+        <v>W12L12</v>
+      </c>
+      <c r="B92" s="1">
+        <f t="shared" si="64"/>
+        <v>12</v>
+      </c>
+      <c r="C92" s="1">
+        <f t="shared" si="65"/>
+        <v>12</v>
+      </c>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1">
+        <f t="shared" si="66"/>
+        <v>12</v>
+      </c>
+      <c r="F92" s="1">
+        <f t="shared" si="67"/>
+        <v>16</v>
+      </c>
+      <c r="G92" s="1">
+        <f t="shared" si="68"/>
+        <v>12</v>
+      </c>
+      <c r="H92" s="1">
+        <f t="shared" si="69"/>
+        <v>16</v>
+      </c>
+      <c r="I92" s="1" t="str">
+        <f t="shared" si="70"/>
+        <v>+'W12L12 12 12  12 16 12 16 \r\n'</v>
+      </c>
+      <c r="J92" s="1">
+        <f t="shared" si="71"/>
+        <v>144</v>
+      </c>
+      <c r="K92" s="1">
+        <f t="shared" si="72"/>
+        <v>192</v>
+      </c>
+      <c r="L92" s="1">
+        <f t="shared" si="73"/>
+        <v>192</v>
+      </c>
+      <c r="M92" s="1">
+        <f t="shared" si="74"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
+      <c r="K93" s="1"/>
+      <c r="L93" s="1"/>
+      <c r="M93" s="1"/>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+      <c r="L94" s="1"/>
+      <c r="M94" s="1"/>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+      <c r="K95" s="1"/>
+      <c r="L95" s="1"/>
+      <c r="M95" s="1"/>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+      <c r="K96" s="1"/>
+      <c r="L96" s="1"/>
+      <c r="M96" s="1"/>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+      <c r="L97" s="1"/>
+      <c r="M97" s="1"/>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+      <c r="K98" s="1"/>
+      <c r="L98" s="1"/>
+      <c r="M98" s="1"/>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
+      <c r="K99" s="1"/>
+      <c r="L99" s="1"/>
+      <c r="M99" s="1"/>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+      <c r="J100" s="1"/>
+      <c r="K100" s="1"/>
+      <c r="L100" s="1"/>
+      <c r="M100" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:C1048576">

</xml_diff>